<commit_message>
Start of Section 3
</commit_message>
<xml_diff>
--- a/Study Plan for Fullstack App.xlsx
+++ b/Study Plan for Fullstack App.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t xml:space="preserve">Priority</t>
   </si>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t xml:space="preserve">Section 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In Progress</t>
   </si>
   <si>
     <t xml:space="preserve">Section 3</t>
@@ -692,7 +689,7 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="20.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.94"/>
@@ -731,15 +728,15 @@
       </c>
       <c r="D2" s="6" t="n">
         <f aca="false">SUM(FIN_ESTIMATES)</f>
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="6" t="n">
         <f aca="false">SUM(DAYS_LEFT)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" s="7" t="n">
         <f aca="false">COUNTIF(STATUSES,"Done")/(COUNTIF(STATUSES,"Not Started")+COUNTIF(STATUSES,"In Progress")+COUNTIF(STATUSES,"Done"))</f>
-        <v>0.0454545454545455</v>
+        <v>0.0909090909090909</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -753,15 +750,15 @@
       </c>
       <c r="D3" s="11" t="n">
         <f aca="false">SUM(D2:D2)</f>
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="E3" s="12" t="n">
         <f aca="false">SUM(E2:E2)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" s="13" t="n">
         <f aca="false">(D3-E3)/D3</f>
-        <v>0.555555555555556</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,15 +772,15 @@
       </c>
       <c r="D4" s="17" t="n">
         <f aca="false">SUM(D2:D2)</f>
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="E4" s="18" t="n">
         <f aca="false">SUM(E2:E2)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4" s="19" t="n">
         <f aca="false">(D4-E4)/D4</f>
-        <v>0.555555555555556</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -827,11 +824,11 @@
       </c>
       <c r="D8" s="26" t="n">
         <f aca="true">MAX(0,(B8-NOW()+1)/7*2)</f>
-        <v>4.92682099781814</v>
+        <v>4.86548550648981</v>
       </c>
       <c r="E8" s="26" t="n">
         <f aca="false">SUM(C8:D8)</f>
-        <v>17.783963854961</v>
+        <v>17.7226283636327</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -864,11 +861,11 @@
       </c>
       <c r="B12" s="28" t="str">
         <f aca="false">ROUND(TOTAL_PLUS_EXTRA_TIME_SPENT/(DEADLINE-STARTDATE+1),1) &amp; " h/day"</f>
-        <v>0.3 h/day</v>
+        <v>0.4 h/day</v>
       </c>
       <c r="C12" s="28" t="str">
         <f aca="false">IF(TOTAL_DAYS_LEFT = 0, "N/A", ROUND(TOTAL_EXTRA_WORK_HOURS_LEFT/TOTAL_DAYS_LEFT,1) &amp; " h/day")</f>
-        <v>0.1 h/day</v>
+        <v>0 h/day</v>
       </c>
       <c r="D12" s="28" t="e">
         <f aca="true">IF(TODAY()&gt;DEADLINE, "N/A", ROUND((TOTAL_PLUS_EXTRA_TIME_SPENT-TOTAL_EXTRA_WORK_HOURS_LEFT)/(TODAY()-STARTDATE+1),1) &amp; " h/day")</f>
@@ -930,14 +927,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="15.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.75"/>
   </cols>
@@ -997,14 +994,14 @@
         <v>3.5</v>
       </c>
       <c r="C5" s="33" t="n">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="D5" s="34" t="n">
         <f aca="false">IF(E5 = "Done",0,C5)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H5" s="35"/>
       <c r="I5" s="36"/>
@@ -1029,226 +1026,226 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="31"/>
       <c r="G7" s="32"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="31"/>
       <c r="G13" s="32"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="33" t="n">
         <v>3.5</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1312,24 +1309,24 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="93.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>